<commit_message>
fix: update OCR models and response handling
Co-Authored-By: Paul Weng <dumessi@icloud.com>
</commit_message>
<xml_diff>
--- a/tests/test_data/test_order.xlsx
+++ b/tests/test_data/test_order.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,116 +436,82 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>序号</t>
+          <t>material_name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>物料名称</t>
+          <t>specification</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>规格型号</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>单位</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>数量</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>连接方式</t>
+          <t>unit</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>卡箍</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>卡箍</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>DN100</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>个</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>钢卡</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>沟槽大小头</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>沟槽大小头</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>DN100*80</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>个</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>14</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>卡簧</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>沟槽弯头</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>沟槽弯头</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>DN80*65</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>个</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>14</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>卡簧</t>
         </is>
       </c>
     </row>

</xml_diff>